<commit_message>
[UPDATE] My frist paper ver. 1.
</commit_message>
<xml_diff>
--- a/result/bM_phi_all_best.xlsx
+++ b/result/bM_phi_all_best.xlsx
@@ -7182,7 +7182,7 @@
         </is>
       </c>
       <c r="B675" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="676">
@@ -7192,7 +7192,7 @@
         </is>
       </c>
       <c r="B676" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="677">
@@ -7202,7 +7202,7 @@
         </is>
       </c>
       <c r="B677" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="678">
@@ -7212,7 +7212,7 @@
         </is>
       </c>
       <c r="B678" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="679">
@@ -7222,7 +7222,7 @@
         </is>
       </c>
       <c r="B679" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="680">
@@ -7232,7 +7232,7 @@
         </is>
       </c>
       <c r="B680" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="681">
@@ -7242,7 +7242,7 @@
         </is>
       </c>
       <c r="B681" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="682">
@@ -7252,7 +7252,7 @@
         </is>
       </c>
       <c r="B682" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="683">
@@ -7262,7 +7262,7 @@
         </is>
       </c>
       <c r="B683" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="684">
@@ -7272,7 +7272,7 @@
         </is>
       </c>
       <c r="B684" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="685">
@@ -7282,7 +7282,7 @@
         </is>
       </c>
       <c r="B685" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="686">
@@ -7292,7 +7292,7 @@
         </is>
       </c>
       <c r="B686" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="687">
@@ -7302,7 +7302,7 @@
         </is>
       </c>
       <c r="B687" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="688">
@@ -7312,7 +7312,7 @@
         </is>
       </c>
       <c r="B688" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="689">
@@ -7322,7 +7322,7 @@
         </is>
       </c>
       <c r="B689" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="690">
@@ -7332,7 +7332,7 @@
         </is>
       </c>
       <c r="B690" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="691">
@@ -7342,7 +7342,7 @@
         </is>
       </c>
       <c r="B691" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="692">
@@ -7352,7 +7352,7 @@
         </is>
       </c>
       <c r="B692" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="693">
@@ -7362,7 +7362,7 @@
         </is>
       </c>
       <c r="B693" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="694">
@@ -7372,7 +7372,7 @@
         </is>
       </c>
       <c r="B694" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="695">
@@ -7382,7 +7382,7 @@
         </is>
       </c>
       <c r="B695" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="696">
@@ -7392,7 +7392,7 @@
         </is>
       </c>
       <c r="B696" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="697">
@@ -7402,7 +7402,7 @@
         </is>
       </c>
       <c r="B697" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="698">
@@ -7412,7 +7412,7 @@
         </is>
       </c>
       <c r="B698" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="699">
@@ -7422,7 +7422,7 @@
         </is>
       </c>
       <c r="B699" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="700">
@@ -7432,7 +7432,7 @@
         </is>
       </c>
       <c r="B700" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="701">
@@ -7442,7 +7442,7 @@
         </is>
       </c>
       <c r="B701" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="702">
@@ -7452,7 +7452,7 @@
         </is>
       </c>
       <c r="B702" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="703">
@@ -7462,7 +7462,7 @@
         </is>
       </c>
       <c r="B703" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="704">
@@ -7472,7 +7472,7 @@
         </is>
       </c>
       <c r="B704" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="705">
@@ -7482,7 +7482,7 @@
         </is>
       </c>
       <c r="B705" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="706">
@@ -7492,7 +7492,7 @@
         </is>
       </c>
       <c r="B706" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="707">
@@ -7502,7 +7502,7 @@
         </is>
       </c>
       <c r="B707" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="708">
@@ -7512,7 +7512,7 @@
         </is>
       </c>
       <c r="B708" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="709">
@@ -7522,7 +7522,7 @@
         </is>
       </c>
       <c r="B709" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="710">
@@ -7532,7 +7532,7 @@
         </is>
       </c>
       <c r="B710" t="n">
-        <v>-0.005</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="711">
@@ -7542,7 +7542,7 @@
         </is>
       </c>
       <c r="B711" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="712">
@@ -7552,7 +7552,7 @@
         </is>
       </c>
       <c r="B712" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="713">
@@ -7562,7 +7562,7 @@
         </is>
       </c>
       <c r="B713" t="n">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="714">
@@ -7572,7 +7572,7 @@
         </is>
       </c>
       <c r="B714" t="n">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="715">
@@ -7582,7 +7582,7 @@
         </is>
       </c>
       <c r="B715" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="716">
@@ -7592,7 +7592,7 @@
         </is>
       </c>
       <c r="B716" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="717">
@@ -7602,7 +7602,7 @@
         </is>
       </c>
       <c r="B717" t="n">
-        <v>-0.005</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="718">
@@ -7612,7 +7612,7 @@
         </is>
       </c>
       <c r="B718" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="719">
@@ -7622,7 +7622,7 @@
         </is>
       </c>
       <c r="B719" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="720">
@@ -7632,7 +7632,7 @@
         </is>
       </c>
       <c r="B720" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="721">
@@ -7642,7 +7642,7 @@
         </is>
       </c>
       <c r="B721" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="722">
@@ -7652,7 +7652,7 @@
         </is>
       </c>
       <c r="B722" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="723">
@@ -7662,7 +7662,7 @@
         </is>
       </c>
       <c r="B723" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="724">
@@ -7672,7 +7672,7 @@
         </is>
       </c>
       <c r="B724" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="725">
@@ -7682,7 +7682,7 @@
         </is>
       </c>
       <c r="B725" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="726">
@@ -7692,7 +7692,7 @@
         </is>
       </c>
       <c r="B726" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="727">
@@ -7702,7 +7702,7 @@
         </is>
       </c>
       <c r="B727" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="728">
@@ -7712,7 +7712,7 @@
         </is>
       </c>
       <c r="B728" t="n">
-        <v>0.005000000000000001</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="729">
@@ -7722,7 +7722,7 @@
         </is>
       </c>
       <c r="B729" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="730">
@@ -7732,7 +7732,7 @@
         </is>
       </c>
       <c r="B730" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="731">
@@ -7742,7 +7742,7 @@
         </is>
       </c>
       <c r="B731" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="732">
@@ -7752,7 +7752,7 @@
         </is>
       </c>
       <c r="B732" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="733">
@@ -7762,7 +7762,7 @@
         </is>
       </c>
       <c r="B733" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="734">
@@ -7772,7 +7772,7 @@
         </is>
       </c>
       <c r="B734" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="735">
@@ -7782,7 +7782,7 @@
         </is>
       </c>
       <c r="B735" t="n">
-        <v>0.005000000000000001</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="736">
@@ -7792,7 +7792,7 @@
         </is>
       </c>
       <c r="B736" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="737">
@@ -7802,7 +7802,7 @@
         </is>
       </c>
       <c r="B737" t="n">
-        <v>-0.004999999999999893</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="738">
@@ -7812,7 +7812,7 @@
         </is>
       </c>
       <c r="B738" t="n">
-        <v>0.005000000000000004</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="739">
@@ -7822,7 +7822,7 @@
         </is>
       </c>
       <c r="B739" t="n">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="740">
@@ -7832,7 +7832,7 @@
         </is>
       </c>
       <c r="B740" t="n">
-        <v>-0.004999999999999893</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="741">
@@ -7842,7 +7842,7 @@
         </is>
       </c>
       <c r="B741" t="n">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="742">
@@ -7852,7 +7852,7 @@
         </is>
       </c>
       <c r="B742" t="n">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="743">
@@ -7862,7 +7862,7 @@
         </is>
       </c>
       <c r="B743" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="744">
@@ -7872,7 +7872,7 @@
         </is>
       </c>
       <c r="B744" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="745">
@@ -7882,7 +7882,7 @@
         </is>
       </c>
       <c r="B745" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="746">
@@ -7892,7 +7892,7 @@
         </is>
       </c>
       <c r="B746" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="747">
@@ -7902,7 +7902,7 @@
         </is>
       </c>
       <c r="B747" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="748">
@@ -7912,7 +7912,7 @@
         </is>
       </c>
       <c r="B748" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03000000000000001</v>
       </c>
     </row>
     <row r="749">
@@ -7922,7 +7922,7 @@
         </is>
       </c>
       <c r="B749" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="750">
@@ -7932,7 +7932,7 @@
         </is>
       </c>
       <c r="B750" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="751">
@@ -7942,7 +7942,7 @@
         </is>
       </c>
       <c r="B751" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="752">
@@ -7952,7 +7952,7 @@
         </is>
       </c>
       <c r="B752" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="753">
@@ -7962,7 +7962,7 @@
         </is>
       </c>
       <c r="B753" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="754">
@@ -7972,7 +7972,7 @@
         </is>
       </c>
       <c r="B754" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="755">
@@ -7982,7 +7982,7 @@
         </is>
       </c>
       <c r="B755" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="756">
@@ -7992,7 +7992,7 @@
         </is>
       </c>
       <c r="B756" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="757">
@@ -8002,7 +8002,7 @@
         </is>
       </c>
       <c r="B757" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="758">
@@ -8012,7 +8012,7 @@
         </is>
       </c>
       <c r="B758" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="759">
@@ -8022,7 +8022,7 @@
         </is>
       </c>
       <c r="B759" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="760">
@@ -8032,7 +8032,7 @@
         </is>
       </c>
       <c r="B760" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="761">
@@ -8042,7 +8042,7 @@
         </is>
       </c>
       <c r="B761" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="762">
@@ -8052,7 +8052,7 @@
         </is>
       </c>
       <c r="B762" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="763">
@@ -8062,7 +8062,7 @@
         </is>
       </c>
       <c r="B763" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="764">
@@ -8072,7 +8072,7 @@
         </is>
       </c>
       <c r="B764" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="765">
@@ -8082,7 +8082,7 @@
         </is>
       </c>
       <c r="B765" t="n">
-        <v>-0.004999999999999998</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="766">
@@ -8092,7 +8092,7 @@
         </is>
       </c>
       <c r="B766" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="767">
@@ -8102,7 +8102,7 @@
         </is>
       </c>
       <c r="B767" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="768">
@@ -8112,7 +8112,7 @@
         </is>
       </c>
       <c r="B768" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="769">
@@ -8122,7 +8122,7 @@
         </is>
       </c>
       <c r="B769" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="770">
@@ -8132,7 +8132,7 @@
         </is>
       </c>
       <c r="B770" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="771">
@@ -8142,7 +8142,7 @@
         </is>
       </c>
       <c r="B771" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="772">
@@ -8152,7 +8152,7 @@
         </is>
       </c>
       <c r="B772" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="773">
@@ -8162,7 +8162,7 @@
         </is>
       </c>
       <c r="B773" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="774">
@@ -8172,7 +8172,7 @@
         </is>
       </c>
       <c r="B774" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="775">
@@ -8182,7 +8182,7 @@
         </is>
       </c>
       <c r="B775" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="776">
@@ -8192,7 +8192,7 @@
         </is>
       </c>
       <c r="B776" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="777">
@@ -8202,7 +8202,7 @@
         </is>
       </c>
       <c r="B777" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="778">
@@ -8212,7 +8212,7 @@
         </is>
       </c>
       <c r="B778" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="779">
@@ -8222,7 +8222,7 @@
         </is>
       </c>
       <c r="B779" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="780">
@@ -8232,7 +8232,7 @@
         </is>
       </c>
       <c r="B780" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="781">
@@ -8242,7 +8242,7 @@
         </is>
       </c>
       <c r="B781" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="782">
@@ -8252,7 +8252,7 @@
         </is>
       </c>
       <c r="B782" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="783">
@@ -8262,7 +8262,7 @@
         </is>
       </c>
       <c r="B783" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="784">
@@ -8272,7 +8272,7 @@
         </is>
       </c>
       <c r="B784" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="785">
@@ -8282,7 +8282,7 @@
         </is>
       </c>
       <c r="B785" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="786">
@@ -8292,7 +8292,7 @@
         </is>
       </c>
       <c r="B786" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="787">
@@ -8302,7 +8302,7 @@
         </is>
       </c>
       <c r="B787" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="788">
@@ -8312,7 +8312,7 @@
         </is>
       </c>
       <c r="B788" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="789">
@@ -8322,7 +8322,7 @@
         </is>
       </c>
       <c r="B789" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="790">
@@ -8332,7 +8332,7 @@
         </is>
       </c>
       <c r="B790" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="791">
@@ -8342,7 +8342,7 @@
         </is>
       </c>
       <c r="B791" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="792">
@@ -8352,7 +8352,7 @@
         </is>
       </c>
       <c r="B792" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="793">
@@ -8362,7 +8362,7 @@
         </is>
       </c>
       <c r="B793" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="794">
@@ -8372,7 +8372,7 @@
         </is>
       </c>
       <c r="B794" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="795">
@@ -8382,7 +8382,7 @@
         </is>
       </c>
       <c r="B795" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="796">
@@ -8392,7 +8392,7 @@
         </is>
       </c>
       <c r="B796" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="797">
@@ -8402,7 +8402,7 @@
         </is>
       </c>
       <c r="B797" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="798">
@@ -8412,7 +8412,7 @@
         </is>
       </c>
       <c r="B798" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="799">
@@ -8422,7 +8422,7 @@
         </is>
       </c>
       <c r="B799" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="800">
@@ -8432,7 +8432,7 @@
         </is>
       </c>
       <c r="B800" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="801">
@@ -8442,7 +8442,7 @@
         </is>
       </c>
       <c r="B801" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="802">
@@ -8452,7 +8452,7 @@
         </is>
       </c>
       <c r="B802" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="803">
@@ -8462,7 +8462,7 @@
         </is>
       </c>
       <c r="B803" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="804">
@@ -8472,7 +8472,7 @@
         </is>
       </c>
       <c r="B804" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="805">
@@ -8482,7 +8482,7 @@
         </is>
       </c>
       <c r="B805" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="806">
@@ -8492,7 +8492,7 @@
         </is>
       </c>
       <c r="B806" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="807">
@@ -8502,7 +8502,7 @@
         </is>
       </c>
       <c r="B807" t="n">
-        <v>0.005</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="808">
@@ -8512,7 +8512,7 @@
         </is>
       </c>
       <c r="B808" t="n">
-        <v>0.005</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="809">
@@ -8522,7 +8522,7 @@
         </is>
       </c>
       <c r="B809" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="810">
@@ -8532,7 +8532,7 @@
         </is>
       </c>
       <c r="B810" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="811">
@@ -8542,7 +8542,7 @@
         </is>
       </c>
       <c r="B811" t="n">
-        <v>0.005</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="812">
@@ -8552,7 +8552,7 @@
         </is>
       </c>
       <c r="B812" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="813">
@@ -8562,7 +8562,7 @@
         </is>
       </c>
       <c r="B813" t="n">
-        <v>0.005000000000000004</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="814">
@@ -8572,7 +8572,7 @@
         </is>
       </c>
       <c r="B814" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="815">
@@ -8582,7 +8582,7 @@
         </is>
       </c>
       <c r="B815" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="816">
@@ -8592,7 +8592,7 @@
         </is>
       </c>
       <c r="B816" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="817">
@@ -8602,7 +8602,7 @@
         </is>
       </c>
       <c r="B817" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="818">
@@ -8612,7 +8612,7 @@
         </is>
       </c>
       <c r="B818" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="819">
@@ -8622,7 +8622,7 @@
         </is>
       </c>
       <c r="B819" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="820">
@@ -8632,7 +8632,7 @@
         </is>
       </c>
       <c r="B820" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="821">
@@ -8642,7 +8642,7 @@
         </is>
       </c>
       <c r="B821" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="822">
@@ -8652,7 +8652,7 @@
         </is>
       </c>
       <c r="B822" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="823">
@@ -8662,7 +8662,7 @@
         </is>
       </c>
       <c r="B823" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="824">
@@ -8672,7 +8672,7 @@
         </is>
       </c>
       <c r="B824" t="n">
-        <v>-0.004999999999999893</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="825">
@@ -8682,7 +8682,7 @@
         </is>
       </c>
       <c r="B825" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="826">
@@ -8692,7 +8692,7 @@
         </is>
       </c>
       <c r="B826" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="827">
@@ -8702,7 +8702,7 @@
         </is>
       </c>
       <c r="B827" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="828">
@@ -8712,7 +8712,7 @@
         </is>
       </c>
       <c r="B828" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="829">
@@ -8722,7 +8722,7 @@
         </is>
       </c>
       <c r="B829" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="830">
@@ -8732,7 +8732,7 @@
         </is>
       </c>
       <c r="B830" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="831">
@@ -8742,7 +8742,7 @@
         </is>
       </c>
       <c r="B831" t="n">
-        <v>-0.004999999999999893</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="832">
@@ -8752,7 +8752,7 @@
         </is>
       </c>
       <c r="B832" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="833">
@@ -8762,7 +8762,7 @@
         </is>
       </c>
       <c r="B833" t="n">
-        <v>0.005</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="834">
@@ -8772,7 +8772,7 @@
         </is>
       </c>
       <c r="B834" t="n">
-        <v>-0.005000000000000001</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="835">
@@ -8782,7 +8782,7 @@
         </is>
       </c>
       <c r="B835" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="836">
@@ -8792,7 +8792,7 @@
         </is>
       </c>
       <c r="B836" t="n">
-        <v>0.005</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="837">
@@ -8802,7 +8802,7 @@
         </is>
       </c>
       <c r="B837" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="838">
@@ -8812,7 +8812,7 @@
         </is>
       </c>
       <c r="B838" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="839">
@@ -8822,7 +8822,7 @@
         </is>
       </c>
       <c r="B839" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="840">
@@ -8832,7 +8832,7 @@
         </is>
       </c>
       <c r="B840" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="841">
@@ -8842,7 +8842,7 @@
         </is>
       </c>
       <c r="B841" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="842">
@@ -8852,7 +8852,7 @@
         </is>
       </c>
       <c r="B842" t="n">
-        <v>0.005000000000000004</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="843">
@@ -8862,7 +8862,7 @@
         </is>
       </c>
       <c r="B843" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="844">
@@ -8872,7 +8872,7 @@
         </is>
       </c>
       <c r="B844" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="845">
@@ -8882,7 +8882,7 @@
         </is>
       </c>
       <c r="B845" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="846">
@@ -8892,7 +8892,7 @@
         </is>
       </c>
       <c r="B846" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="847">
@@ -8902,7 +8902,7 @@
         </is>
       </c>
       <c r="B847" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="848">
@@ -8912,7 +8912,7 @@
         </is>
       </c>
       <c r="B848" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="849">
@@ -8922,7 +8922,7 @@
         </is>
       </c>
       <c r="B849" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="850">
@@ -8932,7 +8932,7 @@
         </is>
       </c>
       <c r="B850" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="851">
@@ -8942,7 +8942,7 @@
         </is>
       </c>
       <c r="B851" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="852">
@@ -8952,7 +8952,7 @@
         </is>
       </c>
       <c r="B852" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="853">
@@ -8962,7 +8962,7 @@
         </is>
       </c>
       <c r="B853" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="854">
@@ -8972,7 +8972,7 @@
         </is>
       </c>
       <c r="B854" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="855">
@@ -8982,7 +8982,7 @@
         </is>
       </c>
       <c r="B855" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="856">
@@ -8992,7 +8992,7 @@
         </is>
       </c>
       <c r="B856" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="857">
@@ -9002,7 +9002,7 @@
         </is>
       </c>
       <c r="B857" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="858">
@@ -9012,7 +9012,7 @@
         </is>
       </c>
       <c r="B858" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="859">
@@ -9022,7 +9022,7 @@
         </is>
       </c>
       <c r="B859" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="860">
@@ -9032,7 +9032,7 @@
         </is>
       </c>
       <c r="B860" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="861">
@@ -9042,7 +9042,7 @@
         </is>
       </c>
       <c r="B861" t="n">
-        <v>0.005000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="862">
@@ -9052,7 +9052,7 @@
         </is>
       </c>
       <c r="B862" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="863">
@@ -9062,7 +9062,7 @@
         </is>
       </c>
       <c r="B863" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="864">
@@ -9072,7 +9072,7 @@
         </is>
       </c>
       <c r="B864" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="865">
@@ -9082,7 +9082,7 @@
         </is>
       </c>
       <c r="B865" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="866">
@@ -9092,7 +9092,7 @@
         </is>
       </c>
       <c r="B866" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="867">
@@ -9102,7 +9102,7 @@
         </is>
       </c>
       <c r="B867" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="868">
@@ -9112,7 +9112,7 @@
         </is>
       </c>
       <c r="B868" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="869">
@@ -9122,7 +9122,7 @@
         </is>
       </c>
       <c r="B869" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="870">
@@ -9132,7 +9132,7 @@
         </is>
       </c>
       <c r="B870" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="871">
@@ -9142,7 +9142,7 @@
         </is>
       </c>
       <c r="B871" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="872">
@@ -9152,7 +9152,7 @@
         </is>
       </c>
       <c r="B872" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="873">
@@ -9162,7 +9162,7 @@
         </is>
       </c>
       <c r="B873" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="874">
@@ -9172,7 +9172,7 @@
         </is>
       </c>
       <c r="B874" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="875">
@@ -9182,7 +9182,7 @@
         </is>
       </c>
       <c r="B875" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="876">
@@ -9192,7 +9192,7 @@
         </is>
       </c>
       <c r="B876" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="877">
@@ -9202,7 +9202,7 @@
         </is>
       </c>
       <c r="B877" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="878">
@@ -9212,7 +9212,7 @@
         </is>
       </c>
       <c r="B878" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="879">
@@ -9222,7 +9222,7 @@
         </is>
       </c>
       <c r="B879" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="880">
@@ -9232,7 +9232,7 @@
         </is>
       </c>
       <c r="B880" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="881">
@@ -9242,7 +9242,7 @@
         </is>
       </c>
       <c r="B881" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="882">
@@ -9252,7 +9252,7 @@
         </is>
       </c>
       <c r="B882" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="883">
@@ -9262,7 +9262,7 @@
         </is>
       </c>
       <c r="B883" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="884">
@@ -9272,7 +9272,7 @@
         </is>
       </c>
       <c r="B884" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="885">
@@ -9282,7 +9282,7 @@
         </is>
       </c>
       <c r="B885" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="886">
@@ -9292,7 +9292,7 @@
         </is>
       </c>
       <c r="B886" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="887">
@@ -9302,7 +9302,7 @@
         </is>
       </c>
       <c r="B887" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="888">
@@ -9312,7 +9312,7 @@
         </is>
       </c>
       <c r="B888" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="889">
@@ -9322,7 +9322,7 @@
         </is>
       </c>
       <c r="B889" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="890">
@@ -9332,7 +9332,7 @@
         </is>
       </c>
       <c r="B890" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="891">
@@ -9342,7 +9342,7 @@
         </is>
       </c>
       <c r="B891" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="892">
@@ -9352,7 +9352,7 @@
         </is>
       </c>
       <c r="B892" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="893">
@@ -9362,7 +9362,7 @@
         </is>
       </c>
       <c r="B893" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="894">
@@ -9372,7 +9372,7 @@
         </is>
       </c>
       <c r="B894" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="895">
@@ -9382,7 +9382,7 @@
         </is>
       </c>
       <c r="B895" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="896">
@@ -9842,7 +9842,7 @@
         </is>
       </c>
       <c r="B941" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="942">
@@ -9852,7 +9852,7 @@
         </is>
       </c>
       <c r="B942" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="943">
@@ -9862,7 +9862,7 @@
         </is>
       </c>
       <c r="B943" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="944">
@@ -9872,7 +9872,7 @@
         </is>
       </c>
       <c r="B944" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="945">
@@ -9882,7 +9882,7 @@
         </is>
       </c>
       <c r="B945" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="946">
@@ -9892,7 +9892,7 @@
         </is>
       </c>
       <c r="B946" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="947">
@@ -9902,7 +9902,7 @@
         </is>
       </c>
       <c r="B947" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="948">
@@ -9912,7 +9912,7 @@
         </is>
       </c>
       <c r="B948" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="949">
@@ -9922,7 +9922,7 @@
         </is>
       </c>
       <c r="B949" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="950">
@@ -9932,7 +9932,7 @@
         </is>
       </c>
       <c r="B950" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="951">
@@ -9942,7 +9942,7 @@
         </is>
       </c>
       <c r="B951" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="952">
@@ -9952,7 +9952,7 @@
         </is>
       </c>
       <c r="B952" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="953">
@@ -9962,7 +9962,7 @@
         </is>
       </c>
       <c r="B953" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="954">
@@ -9972,7 +9972,7 @@
         </is>
       </c>
       <c r="B954" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="955">
@@ -9982,7 +9982,7 @@
         </is>
       </c>
       <c r="B955" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="956">
@@ -9992,7 +9992,7 @@
         </is>
       </c>
       <c r="B956" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="957">
@@ -10002,7 +10002,7 @@
         </is>
       </c>
       <c r="B957" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="958">
@@ -10012,7 +10012,7 @@
         </is>
       </c>
       <c r="B958" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="959">
@@ -10022,7 +10022,7 @@
         </is>
       </c>
       <c r="B959" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="960">
@@ -10032,7 +10032,7 @@
         </is>
       </c>
       <c r="B960" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="961">
@@ -10042,7 +10042,7 @@
         </is>
       </c>
       <c r="B961" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="962">
@@ -10052,7 +10052,7 @@
         </is>
       </c>
       <c r="B962" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="963">
@@ -10062,7 +10062,7 @@
         </is>
       </c>
       <c r="B963" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="964">
@@ -10072,7 +10072,7 @@
         </is>
       </c>
       <c r="B964" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="965">
@@ -10082,7 +10082,7 @@
         </is>
       </c>
       <c r="B965" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="966">
@@ -10092,7 +10092,7 @@
         </is>
       </c>
       <c r="B966" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="967">
@@ -10102,7 +10102,7 @@
         </is>
       </c>
       <c r="B967" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="968">
@@ -10112,7 +10112,7 @@
         </is>
       </c>
       <c r="B968" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="969">
@@ -10122,7 +10122,7 @@
         </is>
       </c>
       <c r="B969" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="970">
@@ -10132,7 +10132,7 @@
         </is>
       </c>
       <c r="B970" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="971">
@@ -10142,7 +10142,7 @@
         </is>
       </c>
       <c r="B971" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="972">
@@ -10152,7 +10152,7 @@
         </is>
       </c>
       <c r="B972" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="973">
@@ -10162,7 +10162,7 @@
         </is>
       </c>
       <c r="B973" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="974">
@@ -10172,7 +10172,7 @@
         </is>
       </c>
       <c r="B974" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="975">
@@ -10182,7 +10182,7 @@
         </is>
       </c>
       <c r="B975" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="976">
@@ -10192,7 +10192,7 @@
         </is>
       </c>
       <c r="B976" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="977">
@@ -10202,7 +10202,7 @@
         </is>
       </c>
       <c r="B977" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="978">
@@ -10212,7 +10212,7 @@
         </is>
       </c>
       <c r="B978" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="979">
@@ -10222,7 +10222,7 @@
         </is>
       </c>
       <c r="B979" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="980">
@@ -10232,7 +10232,7 @@
         </is>
       </c>
       <c r="B980" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="981">
@@ -10242,7 +10242,7 @@
         </is>
       </c>
       <c r="B981" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="982">
@@ -10252,7 +10252,7 @@
         </is>
       </c>
       <c r="B982" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="983">
@@ -10262,7 +10262,7 @@
         </is>
       </c>
       <c r="B983" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="984">
@@ -10272,7 +10272,7 @@
         </is>
       </c>
       <c r="B984" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="985">
@@ -10282,7 +10282,7 @@
         </is>
       </c>
       <c r="B985" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="986">
@@ -10292,7 +10292,7 @@
         </is>
       </c>
       <c r="B986" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="987">
@@ -10302,7 +10302,7 @@
         </is>
       </c>
       <c r="B987" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="988">
@@ -10312,7 +10312,7 @@
         </is>
       </c>
       <c r="B988" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="989">
@@ -10322,7 +10322,7 @@
         </is>
       </c>
       <c r="B989" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="990">
@@ -10332,7 +10332,7 @@
         </is>
       </c>
       <c r="B990" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="991">
@@ -10342,7 +10342,7 @@
         </is>
       </c>
       <c r="B991" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="992">
@@ -10352,7 +10352,7 @@
         </is>
       </c>
       <c r="B992" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="993">
@@ -10362,7 +10362,7 @@
         </is>
       </c>
       <c r="B993" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="994">
@@ -10372,7 +10372,7 @@
         </is>
       </c>
       <c r="B994" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="995">
@@ -10382,7 +10382,7 @@
         </is>
       </c>
       <c r="B995" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="996">
@@ -10392,7 +10392,7 @@
         </is>
       </c>
       <c r="B996" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="997">
@@ -10402,7 +10402,7 @@
         </is>
       </c>
       <c r="B997" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="998">
@@ -10412,7 +10412,7 @@
         </is>
       </c>
       <c r="B998" t="n">
-        <v>0.005</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="999">
@@ -10422,7 +10422,7 @@
         </is>
       </c>
       <c r="B999" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1000">
@@ -10432,7 +10432,7 @@
         </is>
       </c>
       <c r="B1000" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1001">
@@ -10442,7 +10442,7 @@
         </is>
       </c>
       <c r="B1001" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1002">
@@ -10452,7 +10452,7 @@
         </is>
       </c>
       <c r="B1002" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1003">
@@ -10462,7 +10462,7 @@
         </is>
       </c>
       <c r="B1003" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1004">
@@ -10472,7 +10472,7 @@
         </is>
       </c>
       <c r="B1004" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1005">
@@ -10482,7 +10482,7 @@
         </is>
       </c>
       <c r="B1005" t="n">
-        <v>0.005</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1006">
@@ -10492,7 +10492,7 @@
         </is>
       </c>
       <c r="B1006" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1007">
@@ -10502,7 +10502,7 @@
         </is>
       </c>
       <c r="B1007" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1008">
@@ -10512,7 +10512,7 @@
         </is>
       </c>
       <c r="B1008" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1009">
@@ -10522,7 +10522,7 @@
         </is>
       </c>
       <c r="B1009" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1010">
@@ -10532,7 +10532,7 @@
         </is>
       </c>
       <c r="B1010" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1011">
@@ -10542,7 +10542,7 @@
         </is>
       </c>
       <c r="B1011" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1012">
@@ -10552,7 +10552,7 @@
         </is>
       </c>
       <c r="B1012" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1013">
@@ -10562,7 +10562,7 @@
         </is>
       </c>
       <c r="B1013" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1014">
@@ -10572,7 +10572,7 @@
         </is>
       </c>
       <c r="B1014" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1015">
@@ -10582,7 +10582,7 @@
         </is>
       </c>
       <c r="B1015" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1016">
@@ -10592,7 +10592,7 @@
         </is>
       </c>
       <c r="B1016" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1017">
@@ -10602,7 +10602,7 @@
         </is>
       </c>
       <c r="B1017" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1018">
@@ -10612,7 +10612,7 @@
         </is>
       </c>
       <c r="B1018" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1019">
@@ -10622,7 +10622,7 @@
         </is>
       </c>
       <c r="B1019" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1020">
@@ -10632,7 +10632,7 @@
         </is>
       </c>
       <c r="B1020" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1021">
@@ -10642,7 +10642,7 @@
         </is>
       </c>
       <c r="B1021" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1022">
@@ -10652,7 +10652,7 @@
         </is>
       </c>
       <c r="B1022" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1023">
@@ -10662,7 +10662,7 @@
         </is>
       </c>
       <c r="B1023" t="n">
-        <v>-0.005000000000000001</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1024">
@@ -10672,7 +10672,7 @@
         </is>
       </c>
       <c r="B1024" t="n">
-        <v>-0.005000000000000001</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1025">
@@ -10682,7 +10682,7 @@
         </is>
       </c>
       <c r="B1025" t="n">
-        <v>0.005</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1026">
@@ -10692,7 +10692,7 @@
         </is>
       </c>
       <c r="B1026" t="n">
-        <v>-0.005000000000000001</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1027">
@@ -10702,7 +10702,7 @@
         </is>
       </c>
       <c r="B1027" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1028">
@@ -10712,7 +10712,7 @@
         </is>
       </c>
       <c r="B1028" t="n">
-        <v>0.005</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="1029">
@@ -10722,7 +10722,7 @@
         </is>
       </c>
       <c r="B1029" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1030">
@@ -10732,7 +10732,7 @@
         </is>
       </c>
       <c r="B1030" t="n">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="1031">
@@ -10742,7 +10742,7 @@
         </is>
       </c>
       <c r="B1031" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="1032">
@@ -10752,7 +10752,7 @@
         </is>
       </c>
       <c r="B1032" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="1033">
@@ -10762,7 +10762,7 @@
         </is>
       </c>
       <c r="B1033" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="1034">
@@ -10772,7 +10772,7 @@
         </is>
       </c>
       <c r="B1034" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="1035">
@@ -10782,7 +10782,7 @@
         </is>
       </c>
       <c r="B1035" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="1036">
@@ -10792,7 +10792,7 @@
         </is>
       </c>
       <c r="B1036" t="n">
-        <v>0.004999999999999998</v>
+        <v>0.03000000000000001</v>
       </c>
     </row>
     <row r="1037">
@@ -10802,7 +10802,7 @@
         </is>
       </c>
       <c r="B1037" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1038">
@@ -10812,7 +10812,7 @@
         </is>
       </c>
       <c r="B1038" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1039">
@@ -10822,7 +10822,7 @@
         </is>
       </c>
       <c r="B1039" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1040">
@@ -10832,7 +10832,7 @@
         </is>
       </c>
       <c r="B1040" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1041">
@@ -10842,7 +10842,7 @@
         </is>
       </c>
       <c r="B1041" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1042">
@@ -10852,7 +10852,7 @@
         </is>
       </c>
       <c r="B1042" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1043">
@@ -10862,7 +10862,7 @@
         </is>
       </c>
       <c r="B1043" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1044">
@@ -10872,7 +10872,7 @@
         </is>
       </c>
       <c r="B1044" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1045">
@@ -10882,7 +10882,7 @@
         </is>
       </c>
       <c r="B1045" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1046">
@@ -10892,7 +10892,7 @@
         </is>
       </c>
       <c r="B1046" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1047">
@@ -10902,7 +10902,7 @@
         </is>
       </c>
       <c r="B1047" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1048">
@@ -10912,7 +10912,7 @@
         </is>
       </c>
       <c r="B1048" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1049">
@@ -10922,7 +10922,7 @@
         </is>
       </c>
       <c r="B1049" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1050">
@@ -10932,7 +10932,7 @@
         </is>
       </c>
       <c r="B1050" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1051">
@@ -10942,7 +10942,7 @@
         </is>
       </c>
       <c r="B1051" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1052">
@@ -10952,7 +10952,7 @@
         </is>
       </c>
       <c r="B1052" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1053">
@@ -10962,7 +10962,7 @@
         </is>
       </c>
       <c r="B1053" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1054">
@@ -10972,7 +10972,7 @@
         </is>
       </c>
       <c r="B1054" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1055">
@@ -10982,7 +10982,7 @@
         </is>
       </c>
       <c r="B1055" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1056">
@@ -10992,7 +10992,7 @@
         </is>
       </c>
       <c r="B1056" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1057">
@@ -11002,7 +11002,7 @@
         </is>
       </c>
       <c r="B1057" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1058">
@@ -11012,7 +11012,7 @@
         </is>
       </c>
       <c r="B1058" t="n">
-        <v>0.004999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1059">
@@ -11312,7 +11312,7 @@
         </is>
       </c>
       <c r="B1088" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1089">
@@ -11322,7 +11322,7 @@
         </is>
       </c>
       <c r="B1089" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1090">
@@ -11332,7 +11332,7 @@
         </is>
       </c>
       <c r="B1090" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1091">
@@ -11342,7 +11342,7 @@
         </is>
       </c>
       <c r="B1091" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1092">
@@ -11352,7 +11352,7 @@
         </is>
       </c>
       <c r="B1092" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1093">
@@ -11362,7 +11362,7 @@
         </is>
       </c>
       <c r="B1093" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1094">
@@ -11372,7 +11372,7 @@
         </is>
       </c>
       <c r="B1094" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1095">
@@ -11702,7 +11702,7 @@
         </is>
       </c>
       <c r="B1127" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1128">
@@ -11712,7 +11712,7 @@
         </is>
       </c>
       <c r="B1128" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1129">
@@ -11722,7 +11722,7 @@
         </is>
       </c>
       <c r="B1129" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1130">
@@ -11732,7 +11732,7 @@
         </is>
       </c>
       <c r="B1130" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1131">
@@ -11742,7 +11742,7 @@
         </is>
       </c>
       <c r="B1131" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1132">
@@ -11752,7 +11752,7 @@
         </is>
       </c>
       <c r="B1132" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="1133">

</xml_diff>